<commit_message>
US-11602: Field balance report: liquidity, details or sum
</commit_message>
<xml_diff>
--- a/bin/addons/vertical_integration/report/field_balance_spec_report_template.xlsx
+++ b/bin/addons/vertical_integration/report/field_balance_spec_report_template.xlsx
@@ -631,7 +631,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="12" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -783,7 +783,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="true"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="true"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -946,8 +946,8 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1146,9 +1146,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1235160</xdr:colOff>
+      <xdr:colOff>1234440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1162,7 +1162,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18000" y="0"/>
-          <a:ext cx="1217160" cy="579600"/>
+          <a:ext cx="1216440" cy="578880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1188,9 +1188,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>316800</xdr:colOff>
+      <xdr:colOff>316080</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1203,8 +1203,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="857520" y="818280"/>
-          <a:ext cx="10658520" cy="3580200"/>
+          <a:off x="859320" y="818280"/>
+          <a:ext cx="10681560" cy="3579480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1226,8 +1226,8 @@
   </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1235,9 +1235,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="25.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="25.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="22.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="14.01"/>
@@ -1885,8 +1885,8 @@
       <c r="AE21" s="7"/>
       <c r="AF21" s="7"/>
     </row>
-    <row r="22" s="87" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="83"/>
+    <row r="22" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="82"/>
       <c r="B22" s="83"/>
       <c r="C22" s="84"/>
       <c r="F22" s="35"/>
@@ -1917,7 +1917,7 @@
       <c r="AE22" s="7"/>
       <c r="AF22" s="7"/>
     </row>
-    <row r="23" s="87" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="89" t="s">
         <v>59</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="K24" s="40"/>
       <c r="L24" s="41"/>
     </row>
-    <row r="25" s="100" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="100" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="91"/>
       <c r="B25" s="92"/>
       <c r="C25" s="93"/>
@@ -1993,7 +1993,10 @@
       <c r="E25" s="95"/>
       <c r="F25" s="88"/>
       <c r="G25" s="36"/>
-      <c r="H25" s="88"/>
+      <c r="H25" s="88" t="n">
+        <f aca="false">SUM(H19:H24)</f>
+        <v>5090.8</v>
+      </c>
       <c r="I25" s="93"/>
       <c r="J25" s="96"/>
       <c r="K25" s="97"/>
@@ -2019,7 +2022,7 @@
       <c r="AE25" s="99"/>
       <c r="AF25" s="99"/>
     </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="68"/>
       <c r="B26" s="66"/>
       <c r="C26" s="38"/>
@@ -2027,10 +2030,7 @@
       <c r="E26" s="34"/>
       <c r="F26" s="35"/>
       <c r="G26" s="69"/>
-      <c r="H26" s="88" t="n">
-        <f aca="false">SUM(H19:H24)</f>
-        <v>5090.8</v>
-      </c>
+      <c r="H26" s="0"/>
       <c r="I26" s="38"/>
       <c r="J26" s="39"/>
       <c r="K26" s="40"/>
@@ -2593,11 +2593,11 @@
   </sheetPr>
   <dimension ref="B27:C34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.83"/>
   </cols>

</xml_diff>

<commit_message>
Never merge field and HQ comment cells
</commit_message>
<xml_diff>
--- a/bin/addons/vertical_integration/report/field_balance_spec_report_template.xlsx
+++ b/bin/addons/vertical_integration/report/field_balance_spec_report_template.xlsx
@@ -589,7 +589,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -652,6 +652,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1150,9 +1154,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1234080</xdr:colOff>
+      <xdr:colOff>1233720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1166,7 +1170,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18000" y="0"/>
-          <a:ext cx="1216080" cy="578520"/>
+          <a:ext cx="1215720" cy="578160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1192,9 +1196,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>315720</xdr:colOff>
+      <xdr:colOff>315360</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1207,8 +1211,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="860040" y="818280"/>
-          <a:ext cx="10688760" cy="3579120"/>
+          <a:off x="860400" y="818280"/>
+          <a:ext cx="10696320" cy="3578760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1230,8 +1234,8 @@
   </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1254,7 +1258,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="33" style="1" width="9.18"/>
   </cols>
   <sheetData>
-    <row r="1" s="18" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="19" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10"/>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -1272,568 +1276,568 @@
       <c r="I1" s="14"/>
       <c r="J1" s="15"/>
       <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="26" t="n">
+      <c r="H2" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="31"/>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="33" t="n">
+      <c r="D3" s="34" t="n">
         <v>44885</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="36" t="s">
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="37" t="n">
+      <c r="H3" s="38" t="n">
         <v>0.9706</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="41"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="42" t="n">
+      <c r="B4" s="43" t="n">
         <v>44865</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36" t="s">
+      <c r="D4" s="44"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="44" t="n">
+      <c r="H4" s="45" t="n">
         <v>1417.076</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="41"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46" t="n">
+      <c r="B5" s="46"/>
+      <c r="C5" s="47" t="n">
         <v>44888</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="37" t="n">
+      <c r="H5" s="38" t="n">
         <v>3003.54</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="41"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="42"/>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="46" t="n">
+      <c r="B6" s="48"/>
+      <c r="C6" s="47" t="n">
         <v>44889</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36" t="s">
+      <c r="D6" s="44"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="44" t="n">
+      <c r="H6" s="45" t="n">
         <v>18</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="41"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="46" t="n">
+      <c r="B7" s="48"/>
+      <c r="C7" s="47" t="n">
         <v>44890</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="41"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="50"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="41"/>
-    </row>
-    <row r="9" s="63" customFormat="true" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="53" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
+    </row>
+    <row r="9" s="64" customFormat="true" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="55" t="s">
+      <c r="B9" s="55"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="59" t="s">
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="60" t="s">
+      <c r="L9" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="61"/>
-      <c r="N9" s="62" t="s">
+      <c r="M9" s="62"/>
+      <c r="N9" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="61"/>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="61"/>
-      <c r="R9" s="61"/>
-      <c r="S9" s="61"/>
-      <c r="T9" s="61"/>
-      <c r="U9" s="61"/>
-      <c r="V9" s="61"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="61"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="61"/>
-      <c r="AB9" s="61"/>
-      <c r="AC9" s="61"/>
-      <c r="AD9" s="61"/>
-      <c r="AE9" s="61"/>
-      <c r="AF9" s="61"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
+      <c r="AC9" s="62"/>
+      <c r="AD9" s="62"/>
+      <c r="AE9" s="62"/>
+      <c r="AF9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24" t="n">
+      <c r="B10" s="52"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25" t="n">
         <v>234223.01</v>
       </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24" t="n">
+      <c r="B11" s="52"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25" t="n">
         <v>345678.89</v>
       </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="41"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67" t="n">
+      <c r="B12" s="67"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68" t="n">
         <v>111.11</v>
       </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="41"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="68"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="41"/>
-    </row>
-    <row r="14" s="63" customFormat="true" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="70" t="s">
+      <c r="A13" s="69"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42"/>
+    </row>
+    <row r="14" s="64" customFormat="true" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="72" t="s">
+      <c r="D14" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="56" t="s">
+      <c r="G14" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="73" t="s">
+      <c r="H14" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="74" t="s">
+      <c r="I14" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="74" t="s">
+      <c r="J14" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="59" t="s">
+      <c r="K14" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="60" t="s">
+      <c r="L14" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="61" t="s">
+      <c r="N14" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="61"/>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
-      <c r="R14" s="61"/>
-      <c r="S14" s="61"/>
-      <c r="T14" s="61"/>
-      <c r="U14" s="61"/>
-      <c r="V14" s="61"/>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="61"/>
-      <c r="AC14" s="61"/>
-      <c r="AD14" s="61"/>
-      <c r="AE14" s="61"/>
-      <c r="AF14" s="61"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="62"/>
+      <c r="U14" s="62"/>
+      <c r="V14" s="62"/>
+      <c r="W14" s="62"/>
+      <c r="X14" s="62"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="62"/>
+      <c r="AC14" s="62"/>
+      <c r="AD14" s="62"/>
+      <c r="AE14" s="62"/>
+      <c r="AF14" s="62"/>
     </row>
     <row r="15" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="34" t="s">
+      <c r="D15" s="44"/>
+      <c r="E15" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="35" t="n">
+      <c r="F15" s="36" t="n">
         <v>2820.99999999953</v>
       </c>
-      <c r="G15" s="69" t="n">
+      <c r="G15" s="70" t="n">
         <v>0.9706</v>
       </c>
-      <c r="H15" s="35" t="n">
+      <c r="H15" s="36" t="n">
         <v>2906.44961879202</v>
       </c>
-      <c r="I15" s="38" t="n">
+      <c r="I15" s="39" t="n">
         <v>0.8</v>
       </c>
-      <c r="J15" s="39" t="n">
+      <c r="J15" s="40" t="n">
         <f aca="false">F15/I15</f>
         <v>3526.24999999942</v>
       </c>
-      <c r="K15" s="40"/>
-      <c r="L15" s="41"/>
-      <c r="N15" s="75" t="s">
+      <c r="K15" s="41"/>
+      <c r="L15" s="42"/>
+      <c r="N15" s="76" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="34" t="s">
+      <c r="D16" s="44"/>
+      <c r="E16" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="35" t="n">
+      <c r="F16" s="36" t="n">
         <v>1637000</v>
       </c>
-      <c r="G16" s="69" t="n">
+      <c r="G16" s="70" t="n">
         <v>3003.54</v>
       </c>
-      <c r="H16" s="35" t="n">
+      <c r="H16" s="36" t="n">
         <v>545.023538890776</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="41"/>
-      <c r="N16" s="76" t="s">
+      <c r="I16" s="39"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="42"/>
+      <c r="N16" s="77" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="68"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="41"/>
-    </row>
-    <row r="18" s="63" customFormat="true" ht="35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="77" t="s">
+      <c r="A17" s="69"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="42"/>
+    </row>
+    <row r="18" s="64" customFormat="true" ht="35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="78" t="s">
+      <c r="C18" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="72" t="s">
+      <c r="D18" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="73" t="s">
+      <c r="F18" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="79" t="s">
+      <c r="G18" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="73" t="s">
+      <c r="H18" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="74" t="s">
+      <c r="I18" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="J18" s="74" t="s">
+      <c r="J18" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="80" t="s">
+      <c r="K18" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="81" t="s">
+      <c r="L18" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61" t="s">
+      <c r="M18" s="62"/>
+      <c r="N18" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="O18" s="61"/>
-      <c r="P18" s="61"/>
-      <c r="Q18" s="61"/>
-      <c r="R18" s="61"/>
-      <c r="S18" s="61"/>
-      <c r="T18" s="61"/>
-      <c r="U18" s="61"/>
-      <c r="V18" s="61"/>
-      <c r="W18" s="61"/>
-      <c r="X18" s="61"/>
-      <c r="Y18" s="61"/>
-      <c r="Z18" s="61"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="62"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="62"/>
+      <c r="W18" s="62"/>
+      <c r="X18" s="62"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="62"/>
+      <c r="AB18" s="62"/>
+      <c r="AC18" s="62"/>
+      <c r="AD18" s="62"/>
+      <c r="AE18" s="62"/>
+      <c r="AF18" s="62"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="43" t="n">
+      <c r="C19" s="39"/>
+      <c r="D19" s="44" t="n">
         <v>44804</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="35" t="n">
+      <c r="F19" s="36" t="n">
         <v>2716</v>
       </c>
-      <c r="G19" s="69" t="n">
+      <c r="G19" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="H19" s="35" t="n">
+      <c r="H19" s="36" t="n">
         <v>2716</v>
       </c>
-      <c r="I19" s="38" t="s">
+      <c r="I19" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="K19" s="40"/>
-      <c r="L19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="42"/>
       <c r="N19" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" s="87" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="82" t="s">
+    <row r="20" s="88" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="84" t="s">
+      <c r="C20" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="43" t="n">
+      <c r="D20" s="44" t="n">
         <v>44808</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="35" t="n">
+      <c r="F20" s="36" t="n">
         <v>1502.87</v>
       </c>
-      <c r="G20" s="69" t="n">
+      <c r="G20" s="70" t="n">
         <v>1.00339836291044</v>
       </c>
-      <c r="H20" s="35" t="n">
+      <c r="H20" s="36" t="n">
         <v>1497.78</v>
       </c>
-      <c r="I20" s="84"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="85"/>
-      <c r="L20" s="86"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="87"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7" t="s">
         <v>58</v>
@@ -1857,17 +1861,17 @@
       <c r="AE20" s="7"/>
       <c r="AF20" s="7"/>
     </row>
-    <row r="21" s="87" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="82"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="84"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="85"/>
-      <c r="L21" s="86"/>
+    <row r="21" s="88" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="83"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="85"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="89"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="87"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
@@ -1889,17 +1893,17 @@
       <c r="AE21" s="7"/>
       <c r="AF21" s="7"/>
     </row>
-    <row r="22" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="82"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="84"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="85"/>
-      <c r="L22" s="86"/>
+    <row r="22" s="88" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="83"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="85"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="87"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
@@ -1921,21 +1925,21 @@
       <c r="AE22" s="7"/>
       <c r="AF22" s="7"/>
     </row>
-    <row r="23" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="89" t="s">
+    <row r="23" s="88" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="83"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="85"/>
-      <c r="L23" s="86"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="87"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
@@ -1958,377 +1962,377 @@
       <c r="AF23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="43" t="n">
+      <c r="D24" s="44" t="n">
         <v>44808</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="35" t="n">
+      <c r="F24" s="36" t="n">
         <v>880</v>
       </c>
-      <c r="G24" s="69" t="n">
+      <c r="G24" s="70" t="n">
         <v>1.00339787005998</v>
       </c>
-      <c r="H24" s="35" t="n">
+      <c r="H24" s="36" t="n">
         <v>877.02</v>
       </c>
-      <c r="I24" s="91" t="s">
+      <c r="I24" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="J24" s="39"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="41"/>
-    </row>
-    <row r="25" s="101" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="92"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="88" t="n">
+      <c r="J24" s="40"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="42"/>
+    </row>
+    <row r="25" s="102" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="93"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="89" t="n">
         <f aca="false">SUM(H19:H24)</f>
         <v>5090.8</v>
       </c>
-      <c r="I25" s="94"/>
-      <c r="J25" s="97"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="99"/>
-      <c r="M25" s="100"/>
-      <c r="N25" s="100"/>
-      <c r="O25" s="100"/>
-      <c r="P25" s="100"/>
-      <c r="Q25" s="100"/>
-      <c r="R25" s="100"/>
-      <c r="S25" s="100"/>
-      <c r="T25" s="100"/>
-      <c r="U25" s="100"/>
-      <c r="V25" s="100"/>
-      <c r="W25" s="100"/>
-      <c r="X25" s="100"/>
-      <c r="Y25" s="100"/>
-      <c r="Z25" s="100"/>
-      <c r="AA25" s="100"/>
-      <c r="AB25" s="100"/>
-      <c r="AC25" s="100"/>
-      <c r="AD25" s="100"/>
-      <c r="AE25" s="100"/>
-      <c r="AF25" s="100"/>
+      <c r="I25" s="95"/>
+      <c r="J25" s="98"/>
+      <c r="K25" s="99"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="101"/>
+      <c r="N25" s="101"/>
+      <c r="O25" s="101"/>
+      <c r="P25" s="101"/>
+      <c r="Q25" s="101"/>
+      <c r="R25" s="101"/>
+      <c r="S25" s="101"/>
+      <c r="T25" s="101"/>
+      <c r="U25" s="101"/>
+      <c r="V25" s="101"/>
+      <c r="W25" s="101"/>
+      <c r="X25" s="101"/>
+      <c r="Y25" s="101"/>
+      <c r="Z25" s="101"/>
+      <c r="AA25" s="101"/>
+      <c r="AB25" s="101"/>
+      <c r="AC25" s="101"/>
+      <c r="AD25" s="101"/>
+      <c r="AE25" s="101"/>
+      <c r="AF25" s="101"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="68"/>
-      <c r="B26" s="66"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="69"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="70"/>
       <c r="H26" s="0"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="41"/>
-    </row>
-    <row r="27" s="103" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="70" t="s">
+      <c r="I26" s="39"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="42"/>
+    </row>
+    <row r="27" s="104" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="72" t="s">
+      <c r="E27" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="73" t="s">
+      <c r="F27" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="79" t="s">
+      <c r="G27" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="H27" s="73" t="s">
+      <c r="H27" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="I27" s="74" t="s">
+      <c r="I27" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="J27" s="74" t="s">
+      <c r="J27" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="K27" s="59" t="s">
+      <c r="K27" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="L27" s="60" t="s">
+      <c r="L27" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="M27" s="102"/>
-      <c r="N27" s="102"/>
-      <c r="O27" s="102"/>
-      <c r="P27" s="102"/>
-      <c r="Q27" s="102"/>
-      <c r="R27" s="102"/>
-      <c r="S27" s="102"/>
-      <c r="T27" s="102"/>
-      <c r="U27" s="102"/>
-      <c r="V27" s="102"/>
-      <c r="W27" s="102"/>
-      <c r="X27" s="102"/>
-      <c r="Y27" s="102"/>
-      <c r="Z27" s="102"/>
-      <c r="AA27" s="102"/>
-      <c r="AB27" s="102"/>
-      <c r="AC27" s="102"/>
-      <c r="AD27" s="102"/>
-      <c r="AE27" s="102"/>
-      <c r="AF27" s="102"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="103"/>
+      <c r="O27" s="103"/>
+      <c r="P27" s="103"/>
+      <c r="Q27" s="103"/>
+      <c r="R27" s="103"/>
+      <c r="S27" s="103"/>
+      <c r="T27" s="103"/>
+      <c r="U27" s="103"/>
+      <c r="V27" s="103"/>
+      <c r="W27" s="103"/>
+      <c r="X27" s="103"/>
+      <c r="Y27" s="103"/>
+      <c r="Z27" s="103"/>
+      <c r="AA27" s="103"/>
+      <c r="AB27" s="103"/>
+      <c r="AC27" s="103"/>
+      <c r="AD27" s="103"/>
+      <c r="AE27" s="103"/>
+      <c r="AF27" s="103"/>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="68"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="90" t="s">
+      <c r="A28" s="69"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="35" t="n">
+      <c r="F28" s="36"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="36" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="38"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="41"/>
-    </row>
-    <row r="29" s="101" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="92"/>
-      <c r="B29" s="93"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="96"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="88" t="n">
+      <c r="I28" s="39"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="42"/>
+    </row>
+    <row r="29" s="102" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="93"/>
+      <c r="B29" s="94"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="89" t="n">
         <v>0</v>
       </c>
-      <c r="I29" s="94"/>
-      <c r="J29" s="97"/>
-      <c r="K29" s="98"/>
-      <c r="L29" s="99"/>
-      <c r="M29" s="100"/>
-      <c r="N29" s="100"/>
-      <c r="O29" s="100"/>
-      <c r="P29" s="100"/>
-      <c r="Q29" s="100"/>
-      <c r="R29" s="100"/>
-      <c r="S29" s="100"/>
-      <c r="T29" s="100"/>
-      <c r="U29" s="100"/>
-      <c r="V29" s="100"/>
-      <c r="W29" s="100"/>
-      <c r="X29" s="100"/>
-      <c r="Y29" s="100"/>
-      <c r="Z29" s="100"/>
-      <c r="AA29" s="100"/>
-      <c r="AB29" s="100"/>
-      <c r="AC29" s="100"/>
-      <c r="AD29" s="100"/>
-      <c r="AE29" s="100"/>
-      <c r="AF29" s="100"/>
+      <c r="I29" s="95"/>
+      <c r="J29" s="98"/>
+      <c r="K29" s="99"/>
+      <c r="L29" s="100"/>
+      <c r="M29" s="101"/>
+      <c r="N29" s="101"/>
+      <c r="O29" s="101"/>
+      <c r="P29" s="101"/>
+      <c r="Q29" s="101"/>
+      <c r="R29" s="101"/>
+      <c r="S29" s="101"/>
+      <c r="T29" s="101"/>
+      <c r="U29" s="101"/>
+      <c r="V29" s="101"/>
+      <c r="W29" s="101"/>
+      <c r="X29" s="101"/>
+      <c r="Y29" s="101"/>
+      <c r="Z29" s="101"/>
+      <c r="AA29" s="101"/>
+      <c r="AB29" s="101"/>
+      <c r="AC29" s="101"/>
+      <c r="AD29" s="101"/>
+      <c r="AE29" s="101"/>
+      <c r="AF29" s="101"/>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="68"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="41"/>
-    </row>
-    <row r="31" s="103" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="70" t="s">
+      <c r="A30" s="69"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="42"/>
+    </row>
+    <row r="31" s="104" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="104"/>
-      <c r="C31" s="105"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="105"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="105" t="s">
+      <c r="B31" s="105"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="107"/>
+      <c r="E31" s="107"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="108"/>
+      <c r="H31" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="I31" s="108"/>
-      <c r="J31" s="109" t="s">
+      <c r="I31" s="109"/>
+      <c r="J31" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="K31" s="59" t="s">
+      <c r="K31" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="L31" s="60" t="s">
+      <c r="L31" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="M31" s="102"/>
-      <c r="N31" s="102" t="s">
+      <c r="M31" s="103"/>
+      <c r="N31" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="O31" s="102"/>
-      <c r="P31" s="102"/>
-      <c r="Q31" s="102"/>
-      <c r="R31" s="102"/>
-      <c r="S31" s="102"/>
-      <c r="T31" s="102"/>
-      <c r="U31" s="102"/>
-      <c r="V31" s="102"/>
-      <c r="W31" s="102"/>
-      <c r="X31" s="102"/>
-      <c r="Y31" s="102"/>
-      <c r="Z31" s="102"/>
-      <c r="AA31" s="102"/>
-      <c r="AB31" s="102"/>
-      <c r="AC31" s="102"/>
-      <c r="AD31" s="102"/>
-      <c r="AE31" s="102"/>
-      <c r="AF31" s="102"/>
+      <c r="O31" s="103"/>
+      <c r="P31" s="103"/>
+      <c r="Q31" s="103"/>
+      <c r="R31" s="103"/>
+      <c r="S31" s="103"/>
+      <c r="T31" s="103"/>
+      <c r="U31" s="103"/>
+      <c r="V31" s="103"/>
+      <c r="W31" s="103"/>
+      <c r="X31" s="103"/>
+      <c r="Y31" s="103"/>
+      <c r="Z31" s="103"/>
+      <c r="AA31" s="103"/>
+      <c r="AB31" s="103"/>
+      <c r="AC31" s="103"/>
+      <c r="AD31" s="103"/>
+      <c r="AE31" s="103"/>
+      <c r="AF31" s="103"/>
     </row>
     <row r="32" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="66"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="35" t="n">
+      <c r="B32" s="67"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="36" t="n">
         <v>-427.81</v>
       </c>
-      <c r="I32" s="38"/>
-      <c r="J32" s="39" t="n">
+      <c r="I32" s="39"/>
+      <c r="J32" s="40" t="n">
         <v>1055</v>
       </c>
-      <c r="K32" s="40"/>
-      <c r="L32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="42"/>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="68"/>
-      <c r="B33" s="66"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="90" t="s">
+      <c r="A33" s="69"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="35"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="35" t="n">
+      <c r="F33" s="36"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="36" t="n">
         <v>0</v>
       </c>
-      <c r="I33" s="38"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="41"/>
-    </row>
-    <row r="34" s="101" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="92"/>
-      <c r="B34" s="93"/>
-      <c r="C34" s="94"/>
-      <c r="D34" s="95"/>
-      <c r="E34" s="96"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="88" t="n">
+      <c r="I33" s="39"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="42"/>
+    </row>
+    <row r="34" s="102" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="93"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="96"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="89"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="89" t="n">
         <v>-31878.51</v>
       </c>
-      <c r="I34" s="94"/>
-      <c r="J34" s="97"/>
-      <c r="K34" s="98"/>
-      <c r="L34" s="99"/>
-      <c r="M34" s="100"/>
-      <c r="N34" s="100"/>
-      <c r="O34" s="100"/>
-      <c r="P34" s="100"/>
-      <c r="Q34" s="100"/>
-      <c r="R34" s="100"/>
-      <c r="S34" s="100"/>
-      <c r="T34" s="100"/>
-      <c r="U34" s="100"/>
-      <c r="V34" s="100"/>
-      <c r="W34" s="100"/>
-      <c r="X34" s="100"/>
-      <c r="Y34" s="100"/>
-      <c r="Z34" s="100"/>
-      <c r="AA34" s="100"/>
-      <c r="AB34" s="100"/>
-      <c r="AC34" s="100"/>
-      <c r="AD34" s="100"/>
-      <c r="AE34" s="100"/>
-      <c r="AF34" s="100"/>
+      <c r="I34" s="95"/>
+      <c r="J34" s="98"/>
+      <c r="K34" s="99"/>
+      <c r="L34" s="100"/>
+      <c r="M34" s="101"/>
+      <c r="N34" s="101"/>
+      <c r="O34" s="101"/>
+      <c r="P34" s="101"/>
+      <c r="Q34" s="101"/>
+      <c r="R34" s="101"/>
+      <c r="S34" s="101"/>
+      <c r="T34" s="101"/>
+      <c r="U34" s="101"/>
+      <c r="V34" s="101"/>
+      <c r="W34" s="101"/>
+      <c r="X34" s="101"/>
+      <c r="Y34" s="101"/>
+      <c r="Z34" s="101"/>
+      <c r="AA34" s="101"/>
+      <c r="AB34" s="101"/>
+      <c r="AC34" s="101"/>
+      <c r="AD34" s="101"/>
+      <c r="AE34" s="101"/>
+      <c r="AF34" s="101"/>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="68"/>
-      <c r="B35" s="66"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="40"/>
-      <c r="L35" s="41"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="42"/>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="68"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="41"/>
-    </row>
-    <row r="37" s="117" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="110"/>
-      <c r="B37" s="111" t="s">
+      <c r="A36" s="69"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="42"/>
+    </row>
+    <row r="37" s="118" customFormat="true" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="111"/>
+      <c r="B37" s="112" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="112"/>
-      <c r="D37" s="112"/>
-      <c r="E37" s="112"/>
-      <c r="F37" s="112"/>
-      <c r="G37" s="113"/>
-      <c r="H37" s="112"/>
-      <c r="I37" s="114"/>
-      <c r="J37" s="114"/>
-      <c r="K37" s="115"/>
-      <c r="L37" s="116"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="113"/>
+      <c r="G37" s="114"/>
+      <c r="H37" s="113"/>
+      <c r="I37" s="115"/>
+      <c r="J37" s="115"/>
+      <c r="K37" s="116"/>
+      <c r="L37" s="117"/>
     </row>
     <row r="1048338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2570,9 +2574,8 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="K1:L1"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
@@ -2597,11 +2600,11 @@
   </sheetPr>
   <dimension ref="B27:C34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.83"/>
   </cols>

</xml_diff>